<commit_message>
Update documentation of biomass-based H2 datasets.
</commit_message>
<xml_diff>
--- a/premise/data/additional_inventories/lci-hydrogen-wood-gasification.xlsx
+++ b/premise/data/additional_inventories/lci-hydrogen-wood-gasification.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11110"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59E0566F-DD85-6E4D-B34C-924E67EDF89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B19DDBE-ADCA-E742-BF6F-1C0C980A861E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,7 +11,7 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$303</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Tabelle1!$A$1:$H$299</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="57">
   <si>
     <t>Activity</t>
   </si>
@@ -53,9 +53,6 @@
     <t>kilogram</t>
   </si>
   <si>
-    <t>source</t>
-  </si>
-  <si>
     <t>comment</t>
   </si>
   <si>
@@ -152,9 +149,6 @@
     <t>Hydrogen from woody biomass gasification</t>
   </si>
   <si>
-    <t>ELEGANCY project, Techno-environmental assessment of biomass to hydrogen for use in the Swiss transport sector, Karin Treyer, Cristina Antonini et al, 2020, https://doi.org/10.1039/D0SE00222D</t>
-  </si>
-  <si>
     <t>Europe without Switzerland</t>
   </si>
   <si>
@@ -170,12 +164,6 @@
     <t>treatment of wood ash mixture, pure, municipal incineration</t>
   </si>
   <si>
-    <t>entrained flow gasifier with dry biomass (wood chips) from Europe as feedstock.</t>
-  </si>
-  <si>
-    <t>Steam-blown dual fluidized bed gasifier with dry biomass (wood chips) from Europe as feedstock.</t>
-  </si>
-  <si>
     <t>hydrogen production, gaseous, 25 bar, from gasification of woody biomass in entrained flow gasifier, at gasification plant</t>
   </si>
   <si>
@@ -201,6 +189,18 @@
   </si>
   <si>
     <t>carbon dioxide, captured at hydrogen production plant, pre, pipeline 200km, storage 1000m</t>
+  </si>
+  <si>
+    <t>The entrained flow gasifier (EF) with CCS operates under high pressure (40 bar) and elevated temperatures (1623 K), utilizing oxygen as the gasification agent. This technology requires extensive biomass pretreatment, including drying, torrefaction, and pulverization to achieve particle sizes under 0.5 mm. The resulting product gas is rich in carbon monoxide (approximately 60 mol%) and free from hydrocarbons like methane and tar, eliminating the need for tar catalytic reforming. Following gasification, the syngas undergoes a water-gas shift process and is then subjected to CO2 capture using an amine-based absorption process with a capture efficiency of 98%. The captured CO2 is dehydrated and compressed for storage. The EF configuration demonstrates high carbon capture potential, achieving an overall CO2 capture rate of about 98%, but requires significant energy inputs for biomass preparation and system operations​. Source: Antonini, Cristina and Treyer, Karin and Moioli, Emanuele and Bauer, Christian and Schildhauer, Tilman J. and Mazzotti, Marco. Hydrogen from wood gasification with CCS – a techno-environmental analysis of production and use as transport fuel. Sustainable Energy Fuels, 2021. http://dx.doi.org/10.1039/D0SE01637C.</t>
+  </si>
+  <si>
+    <t>The entrained flow gasifier (EF) without CCS also operates at high pressure (40 bar) and elevated temperature (1623 K) using oxygen as the gasification agent. Like its CCS counterpart, it necessitates thorough biomass pretreatment, including drying, torrefaction, and pulverization to achieve particle sizes under 0.5 mm. The syngas produced is rich in carbon monoxide (around 60 mol%) and free from hydrocarbons, eliminating the need for tar reforming or steam methane reforming. After gasification, the syngas passes through a water-gas shift section to increase hydrogen yield. However, without CCS, the CO2 generated during the process is emitted directly. The electricity balance benefits from the lack of a CO2 capture unit, but overall greenhouse gas emissions are slightly positive due to these direct CO2 emissions, offset only partially by the biogenic origin of the CO2. Source: Antonini, Cristina and Treyer, Karin and Moioli, Emanuele and Bauer, Christian and Schildhauer, Tilman J. and Mazzotti, Marco. Hydrogen from wood gasification with CCS – a techno-environmental analysis of production and use as transport fuel. Sustainable Energy Fuels, 2021. http://dx.doi.org/10.1039/D0SE01637C.</t>
+  </si>
+  <si>
+    <t>The heat pipe reformer (HPR) is an indirectly heated gasification technology operating at high pressure (up to 10 bar) with steam as the gasification agent. The system consists of two separate reactors: a gasification reactor and a combustion reactor, connected by heat pipes that transfer heat from the combustion of char and additional biomass to drive the endothermic gasification reactions. The syngas produced is rich in hydrogen (around 44 mol%) but also contains carbon monoxide (26 mol%) and methane (12 mol%), necessitating downstream catalytic reforming and a water-gas shift (WGS) process to increase hydrogen yield. Without CCS, CO2 emissions from the system, including those from the combustion reactor, are released into the atmosphere. While the system benefits from efficient heat integration and nitrogen-free syngas due to the indirect heating, its climate impact remains positive without the additional carbon capture step, as biogenic CO2 from the process is not sequestered. Source: Antonini, Cristina and Treyer, Karin and Moioli, Emanuele and Bauer, Christian and Schildhauer, Tilman J. and Mazzotti, Marco. Hydrogen from wood gasification with CCS – a techno-environmental analysis of production and use as transport fuel. Sustainable Energy Fuels, 2021. http://dx.doi.org/10.1039/D0SE01637C.</t>
+  </si>
+  <si>
+    <t>The heat pipe reformer (HPR) with CCS operates as an indirectly heated gasifier, utilizing steam as the gasification agent and functioning at pressures up to 10 bar. Heat is transferred from the combustion reactor, where char and additional biomass are combusted, to the gasification reactor via heat pipes. The produced syngas, rich in hydrogen (about 44 mol%), contains carbon monoxide (26 mol%) and methane (12 mol%), requiring further processing through catalytic reforming and a water-gas shift (WGS) section to maximize hydrogen output. The HPR system incorporates a pre-combustion CO2 capture unit that efficiently separates CO2 from the syngas using an amine-based absorption process. This setup achieves a CO2 capture rate of approximately 60%, with the captured CO2 dehydrated, compressed, and stored. By sequestering biogenic CO2, the system achieves negative lifecycle greenhouse gas emissions, enhancing its environmental performance while maintaining efficient energy integration.  Source: Antonini, Cristina and Treyer, Karin and Moioli, Emanuele and Bauer, Christian and Schildhauer, Tilman J. and Mazzotti, Marco. Hydrogen from wood gasification with CCS – a techno-environmental analysis of production and use as transport fuel. Sustainable Energy Fuels, 2021. http://dx.doi.org/10.1039/D0SE01637C.</t>
   </si>
 </sst>
 </file>
@@ -550,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H303"/>
+  <dimension ref="A1:H299"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B76" sqref="B76"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -563,10 +563,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
@@ -574,12 +574,12 @@
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B4" s="5">
         <v>1.8132045976445506</v>
@@ -590,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -598,7 +598,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
@@ -614,69 +614,87 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10" t="s">
+        <v>5</v>
+      </c>
+      <c r="F10" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>11</v>
+      <c r="B11">
+        <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B12">
+        <v>7.9363849999999996</v>
+      </c>
+      <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="G11" t="s">
-        <v>4</v>
-      </c>
-      <c r="H11" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>13</v>
-      </c>
       <c r="D12" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
       </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
       <c r="G12" t="s">
-        <v>14</v>
+        <v>25</v>
       </c>
       <c r="H12" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
@@ -684,160 +702,157 @@
         <v>52</v>
       </c>
       <c r="B13">
-        <v>7.9363849999999996</v>
+        <v>10.689909999999999</v>
       </c>
       <c r="C13" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
       </c>
-      <c r="F13" t="s">
-        <v>25</v>
-      </c>
       <c r="G13" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H13" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>56</v>
+        <v>27</v>
       </c>
       <c r="B14">
-        <v>10.689909999999999</v>
+        <v>2.54628E-9</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B15">
-        <v>2.54628E-9</v>
+        <v>15.77786</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
       <c r="B16">
-        <v>15.77786</v>
+        <v>10.284599999999999</v>
       </c>
       <c r="C16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E16" t="s">
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H16" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>10.284599999999999</v>
+        <v>1.841294</v>
       </c>
       <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
         <v>33</v>
       </c>
-      <c r="D17" t="s">
-        <v>41</v>
-      </c>
       <c r="E17" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H17" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="B18">
-        <v>1.841294</v>
+        <v>5.3483199147628007E-10</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>2</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="G18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H18" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>35</v>
-      </c>
-      <c r="B19">
-        <v>5.3483199147628007E-10</v>
+        <v>43</v>
+      </c>
+      <c r="B19" s="6">
+        <v>-2.8615461179087901E-7</v>
       </c>
       <c r="C19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D19" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E19" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H19" t="s">
         <v>36</v>
@@ -845,743 +860,791 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" s="6">
-        <v>-2.8615461179087901E-7</v>
+        <v>41</v>
+      </c>
+      <c r="B20">
+        <v>-7.3980000000000001E-3</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H20" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B21">
-        <v>-7.3980000000000001E-3</v>
-      </c>
-      <c r="C21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" t="s">
-        <v>41</v>
-      </c>
-      <c r="E21" t="s">
-        <v>27</v>
-      </c>
-      <c r="G21" t="s">
-        <v>15</v>
-      </c>
-      <c r="H21" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>50</v>
+      <c r="B22" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>1.8132045976445506</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>21</v>
-      </c>
-      <c r="B24">
-        <v>1.8132045976445506</v>
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B25" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B26" t="s">
-        <v>55</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
-        <v>40</v>
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>47</v>
+        <v>10</v>
+      </c>
+      <c r="C29" t="s">
+        <v>11</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>21</v>
+      </c>
+      <c r="G29" t="s">
+        <v>4</v>
+      </c>
+      <c r="H29" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A30" s="1" t="s">
-        <v>9</v>
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+      <c r="G30" t="s">
+        <v>13</v>
+      </c>
+      <c r="H30" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>10</v>
-      </c>
-      <c r="B31" t="s">
-        <v>11</v>
+        <v>48</v>
+      </c>
+      <c r="B31">
+        <v>18.626139999999999</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="E31" t="s">
+        <v>6</v>
+      </c>
+      <c r="F31" t="s">
+        <v>24</v>
+      </c>
+      <c r="G31" t="s">
+        <v>25</v>
+      </c>
+      <c r="H31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>27</v>
+      </c>
+      <c r="B32">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C32" t="s">
+        <v>28</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F31" t="s">
-        <v>22</v>
-      </c>
-      <c r="G31" t="s">
-        <v>4</v>
-      </c>
-      <c r="H31" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>13</v>
-      </c>
-      <c r="D32" t="s">
-        <v>17</v>
-      </c>
-      <c r="E32" t="s">
-        <v>6</v>
-      </c>
       <c r="G32" t="s">
         <v>14</v>
       </c>
       <c r="H32" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B33">
-        <v>18.626139999999999</v>
+        <v>15.77765</v>
       </c>
       <c r="C33" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D33" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E33" t="s">
         <v>6</v>
       </c>
-      <c r="F33" t="s">
-        <v>25</v>
-      </c>
       <c r="G33" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="B34">
-        <v>2.54628E-9</v>
+        <v>10.284599999999999</v>
       </c>
       <c r="C34" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="D34" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E34" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H34" t="s">
-        <v>30</v>
+        <v>50</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="B35">
-        <v>15.77765</v>
+        <v>1.892684</v>
       </c>
       <c r="C35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="E35" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G35" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H35" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="B36">
-        <v>10.284599999999999</v>
+        <v>5.3483199147628007E-10</v>
       </c>
       <c r="C36" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D36" t="s">
-        <v>41</v>
+        <v>2</v>
       </c>
       <c r="E36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H36" t="s">
-        <v>54</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37">
-        <v>1.892684</v>
+        <v>43</v>
+      </c>
+      <c r="B37" s="6">
+        <v>-2.8615461179087901E-7</v>
       </c>
       <c r="C37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D37" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="E37" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="G37" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H37" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B38">
-        <v>5.3483199147628007E-10</v>
+        <v>-7.3980000000000001E-3</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D38" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="E38" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="G38" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="6">
-        <v>-2.8615461179087901E-7</v>
-      </c>
-      <c r="C39" t="s">
-        <v>29</v>
-      </c>
-      <c r="D39" t="s">
-        <v>41</v>
-      </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-      <c r="G39" t="s">
-        <v>15</v>
-      </c>
-      <c r="H39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>43</v>
-      </c>
-      <c r="B40">
-        <v>-7.3980000000000001E-3</v>
-      </c>
-      <c r="C40" t="s">
-        <v>29</v>
-      </c>
-      <c r="D40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E40" t="s">
-        <v>27</v>
-      </c>
-      <c r="G40" t="s">
-        <v>15</v>
-      </c>
-      <c r="H40" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A42" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>49</v>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1.4983549435621251</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="4">
-        <v>1.4983549435621251</v>
+        <v>3</v>
+      </c>
+      <c r="B43" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B44" t="s">
-        <v>17</v>
+        <v>6</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B45" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>5</v>
-      </c>
-      <c r="B46" t="s">
-        <v>6</v>
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A46" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>8</v>
-      </c>
-      <c r="B48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A49" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="C47" t="s">
+        <v>11</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47" t="s">
+        <v>5</v>
+      </c>
+      <c r="F47" t="s">
+        <v>21</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4</v>
+      </c>
+      <c r="H47" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A48" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
+        <v>16</v>
+      </c>
+      <c r="E48" t="s">
+        <v>6</v>
+      </c>
+      <c r="G48" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+      <c r="B49">
+        <v>1.5237000000000001</v>
+      </c>
+      <c r="C49" t="s">
+        <v>22</v>
+      </c>
+      <c r="D49" t="s">
+        <v>23</v>
+      </c>
+      <c r="E49" t="s">
+        <v>6</v>
+      </c>
+      <c r="F49" t="s">
+        <v>24</v>
+      </c>
+      <c r="G49" t="s">
+        <v>25</v>
+      </c>
+      <c r="H49" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>10</v>
-      </c>
-      <c r="B50" t="s">
-        <v>11</v>
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>19.585570000000001</v>
       </c>
       <c r="C50" t="s">
         <v>12</v>
       </c>
       <c r="D50" t="s">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="E50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G50" t="s">
+        <v>14</v>
+      </c>
+      <c r="H50" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>27</v>
+      </c>
+      <c r="B51">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C51" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" t="s">
+        <v>19</v>
+      </c>
+      <c r="E51" t="s">
         <v>5</v>
       </c>
-      <c r="F50" t="s">
-        <v>22</v>
-      </c>
-      <c r="G50" t="s">
-        <v>4</v>
-      </c>
-      <c r="H50" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A51" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B51">
-        <v>1</v>
-      </c>
-      <c r="C51" t="s">
-        <v>13</v>
-      </c>
-      <c r="D51" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" t="s">
-        <v>6</v>
-      </c>
       <c r="G51" t="s">
         <v>14</v>
       </c>
       <c r="H51" t="s">
-        <v>55</v>
+        <v>29</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="B52">
-        <v>1.5237000000000001</v>
+        <v>15.92628</v>
       </c>
       <c r="C52" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D52" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="E52" t="s">
         <v>6</v>
       </c>
-      <c r="F52" t="s">
-        <v>25</v>
-      </c>
       <c r="G52" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H52" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B53">
-        <v>19.585570000000001</v>
+        <v>11.6966</v>
       </c>
       <c r="C53" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E53" t="s">
         <v>6</v>
       </c>
       <c r="G53" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H53" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="B54">
-        <v>2.54628E-9</v>
+        <v>0</v>
       </c>
       <c r="C54" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D54" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E54" t="s">
-        <v>5</v>
+        <v>17</v>
       </c>
       <c r="G54" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H54" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B55">
-        <v>15.92628</v>
+        <v>5.3483199147628007E-10</v>
       </c>
       <c r="C55" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D55" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E55" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G55" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H55" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="B56">
-        <v>11.6966</v>
+        <v>-1.2439E-2</v>
       </c>
       <c r="C56" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="D56" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E56" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G56" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H56" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A57" t="s">
-        <v>16</v>
-      </c>
-      <c r="B57">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C57" t="s">
-        <v>29</v>
-      </c>
-      <c r="D57" t="s">
-        <v>34</v>
-      </c>
-      <c r="E57" t="s">
-        <v>18</v>
-      </c>
-      <c r="G57" t="s">
-        <v>15</v>
-      </c>
-      <c r="H57" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A58" t="s">
-        <v>35</v>
-      </c>
-      <c r="B58">
-        <v>5.3483199147628007E-10</v>
-      </c>
-      <c r="C58" t="s">
-        <v>29</v>
-      </c>
-      <c r="D58" t="s">
-        <v>42</v>
-      </c>
-      <c r="E58" t="s">
-        <v>5</v>
-      </c>
-      <c r="G58" t="s">
-        <v>15</v>
-      </c>
-      <c r="H58" t="s">
-        <v>36</v>
+      <c r="B58" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>43</v>
+        <v>20</v>
       </c>
       <c r="B59">
-        <v>-1.2439E-2</v>
-      </c>
-      <c r="C59" t="s">
-        <v>29</v>
-      </c>
-      <c r="D59" t="s">
-        <v>41</v>
-      </c>
-      <c r="E59" t="s">
-        <v>27</v>
-      </c>
-      <c r="G59" t="s">
-        <v>15</v>
-      </c>
-      <c r="H59" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>48</v>
+        <v>1.4983549435621251</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>21</v>
-      </c>
-      <c r="B62">
-        <v>1.4983549435621251</v>
+        <v>5</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="B63" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" t="s">
+        <v>10</v>
+      </c>
+      <c r="C65" t="s">
+        <v>11</v>
+      </c>
+      <c r="D65" t="s">
+        <v>1</v>
+      </c>
+      <c r="E65" t="s">
         <v>5</v>
       </c>
-      <c r="B65" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A66" t="s">
-        <v>7</v>
-      </c>
-      <c r="B66" t="s">
-        <v>40</v>
+      <c r="F65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" t="s">
+        <v>4</v>
+      </c>
+      <c r="H65" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A66" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66">
+        <v>1</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>16</v>
+      </c>
+      <c r="E66" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" t="s">
+        <v>13</v>
+      </c>
+      <c r="H66" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>8</v>
-      </c>
-      <c r="B67" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A68" s="1" t="s">
-        <v>9</v>
+        <v>48</v>
+      </c>
+      <c r="B67">
+        <v>21.1966</v>
+      </c>
+      <c r="C67" t="s">
+        <v>22</v>
+      </c>
+      <c r="D67" t="s">
+        <v>23</v>
+      </c>
+      <c r="E67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>24</v>
+      </c>
+      <c r="G67" t="s">
+        <v>25</v>
+      </c>
+      <c r="H67" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68">
+        <v>2.54628E-9</v>
+      </c>
+      <c r="C68" t="s">
+        <v>28</v>
+      </c>
+      <c r="D68" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" t="s">
+        <v>5</v>
+      </c>
+      <c r="G68" t="s">
+        <v>14</v>
+      </c>
+      <c r="H68" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>10</v>
-      </c>
-      <c r="B69" t="s">
-        <v>11</v>
+        <v>30</v>
+      </c>
+      <c r="B69">
+        <v>15.905519999999999</v>
       </c>
       <c r="C69" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="D69" t="s">
-        <v>1</v>
+        <v>39</v>
       </c>
       <c r="E69" t="s">
-        <v>5</v>
-      </c>
-      <c r="F69" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="G69" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="H69" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A70" s="2" t="s">
-        <v>48</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>49</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>11.6966</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>32</v>
       </c>
       <c r="D70" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="E70" t="s">
         <v>6</v>
@@ -1590,245 +1653,150 @@
         <v>14</v>
       </c>
       <c r="H70" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="B71">
-        <v>21.1966</v>
+        <v>0</v>
       </c>
       <c r="C71" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="D71" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="E71" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G71" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="H71" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="B72">
-        <v>2.54628E-9</v>
+        <v>5.3483199147628007E-10</v>
       </c>
       <c r="C72" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D72" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="E72" t="s">
         <v>5</v>
       </c>
       <c r="G72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H72" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B73">
-        <v>15.905519999999999</v>
+        <v>-1.2439E-2</v>
       </c>
       <c r="C73" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D73" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="E73" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="G73" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H73" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A74" t="s">
-        <v>53</v>
-      </c>
-      <c r="B74">
-        <v>11.6966</v>
-      </c>
-      <c r="C74" t="s">
-        <v>33</v>
-      </c>
-      <c r="D74" t="s">
-        <v>41</v>
-      </c>
-      <c r="E74" t="s">
-        <v>6</v>
-      </c>
-      <c r="G74" t="s">
-        <v>15</v>
-      </c>
-      <c r="H74" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A75" t="s">
-        <v>16</v>
-      </c>
-      <c r="B75">
-        <v>0</v>
-      </c>
-      <c r="C75" t="s">
-        <v>29</v>
-      </c>
-      <c r="D75" t="s">
-        <v>34</v>
-      </c>
-      <c r="E75" t="s">
-        <v>18</v>
-      </c>
-      <c r="G75" t="s">
-        <v>15</v>
-      </c>
-      <c r="H75" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A76" t="s">
-        <v>35</v>
-      </c>
-      <c r="B76">
-        <v>5.3483199147628007E-10</v>
-      </c>
-      <c r="C76" t="s">
-        <v>29</v>
-      </c>
-      <c r="D76" t="s">
         <v>42</v>
       </c>
-      <c r="E76" t="s">
-        <v>5</v>
-      </c>
-      <c r="G76" t="s">
-        <v>15</v>
-      </c>
-      <c r="H76" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A77" t="s">
-        <v>43</v>
-      </c>
-      <c r="B77">
-        <v>-1.2439E-2</v>
-      </c>
-      <c r="C77" t="s">
-        <v>29</v>
-      </c>
-      <c r="D77" t="s">
-        <v>41</v>
-      </c>
-      <c r="E77" t="s">
-        <v>27</v>
-      </c>
-      <c r="G77" t="s">
-        <v>15</v>
-      </c>
-      <c r="H77" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" ht="16" x14ac:dyDescent="0.2">
-      <c r="A79" s="1"/>
-      <c r="B79" s="1"/>
-    </row>
-    <row r="86" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="98" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A98" s="1"/>
-      <c r="B98" s="1"/>
-    </row>
-    <row r="105" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A105" s="1"/>
-    </row>
-    <row r="113" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A113" s="1"/>
-      <c r="B113" s="1"/>
-    </row>
-    <row r="120" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A120" s="1"/>
-    </row>
-    <row r="142" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" s="1"/>
-      <c r="B142" s="1"/>
-    </row>
-    <row r="148" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="171" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A171" s="1"/>
-      <c r="B171" s="1"/>
-    </row>
-    <row r="177" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A177" s="1"/>
-    </row>
-    <row r="186" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A186" s="1"/>
-      <c r="B186" s="1"/>
-    </row>
-    <row r="192" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A192" s="1"/>
-    </row>
-    <row r="214" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A214" s="1"/>
-      <c r="B214" s="1"/>
-    </row>
-    <row r="220" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A220" s="1"/>
-    </row>
-    <row r="242" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A242" s="1"/>
-      <c r="B242" s="1"/>
-    </row>
-    <row r="248" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A248" s="1"/>
-    </row>
-    <row r="269" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A269" s="1"/>
-      <c r="B269" s="1"/>
-    </row>
-    <row r="275" spans="1:1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A275" s="1"/>
-    </row>
-    <row r="297" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A297" s="1"/>
-      <c r="B297" s="1"/>
-    </row>
-    <row r="303" spans="1:2" ht="16" x14ac:dyDescent="0.2">
-      <c r="A303" s="1"/>
+    </row>
+    <row r="75" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+    </row>
+    <row r="82" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A82" s="1"/>
+    </row>
+    <row r="94" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+    </row>
+    <row r="101" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A101" s="1"/>
+    </row>
+    <row r="109" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A109" s="1"/>
+      <c r="B109" s="1"/>
+    </row>
+    <row r="116" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A116" s="1"/>
+    </row>
+    <row r="138" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A138" s="1"/>
+      <c r="B138" s="1"/>
+    </row>
+    <row r="144" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A144" s="1"/>
+    </row>
+    <row r="167" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A167" s="1"/>
+      <c r="B167" s="1"/>
+    </row>
+    <row r="173" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A173" s="1"/>
+    </row>
+    <row r="182" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A182" s="1"/>
+      <c r="B182" s="1"/>
+    </row>
+    <row r="188" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A188" s="1"/>
+    </row>
+    <row r="210" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A210" s="1"/>
+      <c r="B210" s="1"/>
+    </row>
+    <row r="216" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A216" s="1"/>
+    </row>
+    <row r="238" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A238" s="1"/>
+      <c r="B238" s="1"/>
+    </row>
+    <row r="244" spans="1:1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A244" s="1"/>
+    </row>
+    <row r="265" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A265" s="1"/>
+      <c r="B265" s="1"/>
+    </row>
+    <row r="271" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A271" s="1"/>
+    </row>
+    <row r="293" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A293" s="1"/>
+      <c r="B293" s="1"/>
+    </row>
+    <row r="299" spans="1:2" ht="16" x14ac:dyDescent="0.2">
+      <c r="A299" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H303" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H299" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>